<commit_message>
PEC4-0001: Corregir formula tabla arbol decision.
</commit_message>
<xml_diff>
--- a/pregunta1/tabla_arbol_decision.xlsx
+++ b/pregunta1/tabla_arbol_decision.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Paso 1" sheetId="1" state="visible" r:id="rId3"/>
@@ -78,15 +78,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -108,12 +108,14 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="13"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -121,12 +123,14 @@
       <color rgb="FFFFFF00"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -134,6 +138,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -141,6 +146,7 @@
       <color rgb="FF158466"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -148,6 +154,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -216,44 +223,44 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -478,348 +485,348 @@
   </sheetPr>
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="12.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="12.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="B12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="A14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="A15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="A16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="A17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="5" t="s">
+      <c r="B24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="C25" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" s="8" t="n">
+      <c r="B25" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C25" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="9" t="n">
         <f aca="false">SUM(B25:C25)</f>
         <v>4</v>
       </c>
-      <c r="F25" s="0" t="n">
-        <f aca="false">(B25+C27)/D28</f>
-        <v>0.5</v>
+      <c r="F25" s="1" t="n">
+        <f aca="false">(B25+C26 + C27)/D28</f>
+        <v>0.75</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="C26" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="D26" s="8" t="n">
+      <c r="A26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="C26" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="D26" s="9" t="n">
         <f aca="false">SUM(B26:C26)</f>
         <v>8</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C27" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="D27" s="8" t="n">
+      <c r="A27" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="D27" s="9" t="n">
         <f aca="false">SUM(B27:C27)</f>
         <v>4</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="8" t="n">
+      <c r="D28" s="9" t="n">
         <f aca="false">SUM(B25:C27)</f>
         <v>16</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="6" t="s">
+      <c r="B31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="C32" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D32" s="8" t="n">
+      <c r="B32" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C32" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="9" t="n">
         <f aca="false">SUM(B32:C32)</f>
         <v>4</v>
       </c>
-      <c r="F32" s="0" t="n">
-        <f aca="false">(B32+C33)/D35</f>
-        <v>0.5</v>
+      <c r="F32" s="1" t="n">
+        <f aca="false">(B32+C33 + C34)/D35</f>
+        <v>0.75</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="C33" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="D33" s="8" t="n">
+      <c r="A33" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="C33" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="D33" s="9" t="n">
         <f aca="false">SUM(B33:C33)</f>
         <v>8</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C34" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="D34" s="8" t="n">
+      <c r="A34" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="D34" s="9" t="n">
         <f aca="false">SUM(B34:C34)</f>
         <v>4</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="8" t="n">
+      <c r="D35" s="9" t="n">
         <f aca="false">SUM(B32:C34)</f>
         <v>16</v>
       </c>
@@ -850,154 +857,154 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="12.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="12.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="6" t="s">
+      <c r="B16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="C17" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="8" t="n">
+      <c r="B17" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C17" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="9" t="n">
         <f aca="false">SUM(B17:C17)</f>
         <v>4</v>
       </c>
-      <c r="F17" s="10" t="n">
+      <c r="F17" s="1" t="n">
         <f aca="false">(B17+C18)/D20</f>
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="D18" s="8" t="n">
+      <c r="A18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="D18" s="9" t="n">
         <f aca="false">SUM(B18:C18)</f>
         <v>4</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="8" t="n">
+      <c r="A19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="9" t="n">
         <f aca="false">SUM(B19:C19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="8" t="n">
+      <c r="D20" s="9" t="n">
         <f aca="false">SUM(B17:C19)</f>
         <v>8</v>
       </c>
@@ -1022,160 +1029,160 @@
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="12.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="12.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="21.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="6" t="s">
+      <c r="B16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="8" t="n">
+      <c r="B17" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="9" t="n">
         <f aca="false">SUM(B17:C17)</f>
         <v>0</v>
       </c>
-      <c r="F17" s="10" t="n">
+      <c r="F17" s="1" t="n">
         <f aca="false">(B18+C19)/D20</f>
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="C18" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="8" t="n">
+      <c r="A18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C18" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="9" t="n">
         <f aca="false">SUM(B18:C18)</f>
         <v>4</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="D19" s="8" t="n">
+      <c r="A19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="D19" s="9" t="n">
         <f aca="false">SUM(B19:C19)</f>
         <v>4</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="8" t="n">
+      <c r="D20" s="9" t="n">
         <f aca="false">SUM(B17:C19)</f>
         <v>8</v>
       </c>

</xml_diff>